<commit_message>
changed feedback report time
</commit_message>
<xml_diff>
--- a/Feedback.xlsx
+++ b/Feedback.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>Please select your gender</t>
   </si>
@@ -37,34 +37,95 @@
     <t>Submitted At</t>
   </si>
   <si>
+    <t>both</t>
+  </si>
+  <si>
+    <t>ww</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Interactivity of exhibit</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
     <t>Female</t>
   </si>
   <si>
-    <t>24</t>
+    <t>Ghjjkk</t>
+  </si>
+  <si>
+    <t>Jkll</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25
+</t>
+  </si>
+  <si>
+    <t>Poor</t>
+  </si>
+  <si>
+    <t>explanation of exhibit</t>
+  </si>
+  <si>
+    <t>Uoopkjhg</t>
+  </si>
+  <si>
+    <t>Uiikj</t>
+  </si>
+  <si>
+    <t>25</t>
   </si>
   <si>
     <t>Knowledge</t>
   </si>
   <si>
-    <t>Good</t>
-  </si>
-  <si>
-    <t>Value for money</t>
-  </si>
-  <si>
-    <t>good</t>
-  </si>
-  <si>
-    <t>Entertainment</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>ssss</t>
-  </si>
-  <si>
-    <t>ghhdsd</t>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t>Quatity of exhibit</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>jhjhjh</t>
+  </si>
+  <si>
+    <t>hhj</t>
+  </si>
+  <si>
+    <t>hhjjh</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>Hj</t>
+  </si>
+  <si>
+    <t>Rtu</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>Op</t>
+  </si>
+  <si>
+    <t>Hf</t>
   </si>
 </sst>
 </file>
@@ -442,7 +503,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="30" customWidth="1"/>
@@ -496,27 +557,27 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="1">
-        <v>45310.16981121528</v>
+        <v>45320.42964043982</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -525,10 +586,140 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1">
+        <v>45320.47926789352</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="1">
-        <v>45310.47044230324</v>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1">
+        <v>45320.479864699075</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="1">
+        <v>45320.489508391205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="1">
+        <v>45320.49206712963</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="1">
+        <v>45320.492871678245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="1">
+        <v>45320.51076020833</v>
       </c>
     </row>
   </sheetData>

</xml_diff>